<commit_message>
Full versions (academic and short) with LaTeX code in vitae::detailed_entries
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5DBE52-4B0C-4C70-A0ED-C1DBDC21FA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB5F3EB-B410-4B71-8C37-CA4D94F1C71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>Journals Include</t>
   </si>
   <si>
-    <t>Editorial Boards</t>
-  </si>
-  <si>
     <t>Colombian Institutions</t>
   </si>
   <si>
@@ -88,15 +85,9 @@
     <t>Theme Issue \textbf{\textit{Voice modulation: from origin and mechanism to social impact}} (\href{https://royalsocietypublishing.org/toc/rstb/2021/376/1840}{\textbf{Parte 1}}, \href{https://royalsocietypublishing.org/toc/rstb/2022/377/1841}{\textbf{Parte 2}})</t>
   </si>
   <si>
-    <t>Editado por Juan David Leongómez, Katarzyna Pisanski, David Reby, Disa Sauter, Nadine Lavan, Marcus Perlman y Jaroslava Varella Valentova</t>
-  </si>
-  <si>
     <t>Specialty section on \href{https://www.frontiersin.org/journals/psychology/sections/evolutionary-psychology}{Evolutionary Psychology}</t>
   </si>
   <si>
-    <t>Perfil \href{https://loop.frontiersin.org/people/438954/overview}{Loop}</t>
-  </si>
-  <si>
     <t>\href{https://royalsocietypublishing.org/journal/rspb}{Proceedings of the Royal Society B: Biological Sciences}</t>
   </si>
   <si>
@@ -137,6 +128,15 @@
   </si>
   <si>
     <t>\href{https://unal.edu.co/}{Universidad Nacional de Colombia}</t>
+  </si>
+  <si>
+    <t>Guest editorial team</t>
+  </si>
+  <si>
+    <t>Edited by Juan David Leongómez, Katarzyna Pisanski, David Reby, Disa Sauter, Nadine Lavan, Marcus Perlman \&amp; Jaroslava Varella Valentova</t>
+  </si>
+  <si>
+    <t>\href{https://loop.frontiersin.org/people/438954/overview}{Loop} profile</t>
   </si>
 </sst>
 </file>
@@ -983,7 +983,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,19 +1014,19 @@
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1046,16 +1046,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,13 +1066,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,7 +1110,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1159,7 +1159,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1202,10 +1202,10 @@
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add PCI RR rols and change {fontawesome} for {fontawesome5}
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB5F3EB-B410-4B71-8C37-CA4D94F1C71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7981E-A71F-4E94-A5C9-56036CEF8A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>what</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t>\href{https://loop.frontiersin.org/people/438954/overview}{Loop} profile</t>
+  </si>
+  <si>
+    <t>Recommender (editor)</t>
+  </si>
+  <si>
+    <t>Since 2023</t>
+  </si>
+  <si>
+    <t>\href{https://rr.peercommunityin.org/}{PCI Registered Reports}</t>
+  </si>
+  <si>
+    <t>Editorial team</t>
+  </si>
+  <si>
+    <t>Recommender</t>
+  </si>
+  <si>
+    <t>Issue Stage 1 and Stage 2 recommendations</t>
+  </si>
+  <si>
+    <t>\href{https://rr.peercommunityin.org/public/user_public_page?userId=1996}{Recommender} profile</t>
   </si>
 </sst>
 </file>
@@ -980,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AFA9E8-48DD-493D-A757-B362F16614DE}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,96 +1033,106 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,7 +1141,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1119,18 +1150,16 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,27 +1168,27 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,7 +1197,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,7 +1208,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,24 +1217,18 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,22 +1237,34 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1245,6 +1280,20 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Biology Letters as reviewer
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7981E-A71F-4E94-A5C9-56036CEF8A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C576C3B3-82AC-4441-9087-F0D1033AF2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>what</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>\href{https://rr.peercommunityin.org/public/user_public_page?userId=1996}{Recommender} profile</t>
+  </si>
+  <si>
+    <t>\href{https://royalsocietypublishing.org/journal/rsbl}{Biology Letters}</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AFA9E8-48DD-493D-A757-B362F16614DE}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1153,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1159,7 +1162,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,27 +1171,27 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,73 +1200,73 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1271,7 +1274,9 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1294,6 +1299,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Replace PCI RR with full name
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C576C3B3-82AC-4441-9087-F0D1033AF2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E973329-E80C-4068-B985-3DD083A6BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>what</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Since 2023</t>
   </si>
   <si>
-    <t>\href{https://rr.peercommunityin.org/}{PCI Registered Reports}</t>
-  </si>
-  <si>
     <t>Editorial team</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>\href{https://royalsocietypublishing.org/journal/rsbl}{Biology Letters}</t>
+  </si>
+  <si>
+    <t>\href{https://rr.peercommunityin.org/}{Peer Community In Registered Reports}</t>
   </si>
 </sst>
 </file>
@@ -708,9 +708,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -748,7 +748,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -854,7 +854,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -996,7 +996,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1004,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3AFA9E8-48DD-493D-A757-B362F16614DE}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1044,13 +1044,13 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1059,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
@@ -1124,27 +1124,27 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1162,7 +1162,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,27 +1180,27 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1209,73 +1209,73 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,9 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1306,6 +1308,13 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Grants as reviewer for UNal and Minciencias
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B2F0D4-E073-448A-91E7-3E4DFDC10EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56340CBF-2C72-46EB-BE0C-4223C2FE7A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25740" yWindow="3720" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26070" yWindow="2730" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>\href{http://sumapsicologica.konradlorenz.edu.co/}{Summa Psicológica}</t>
   </si>
   <si>
-    <t>Publication Evaluation</t>
-  </si>
-  <si>
     <t>Since 2015</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>\href{https://royalsocietypublishing.org/journal/rspb}{Proceedings of the Royal Society B: \newline Biological Sciences}</t>
+  </si>
+  <si>
+    <t>Publication/Grant Evaluation</t>
   </si>
 </sst>
 </file>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -686,24 +686,24 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add review for Peace and Conflict: Journal of Peace Psychology
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>what</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">\href{https://journals.sagepub.com/home/evp}{Evolutionary Psychology}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\href{https://www.apa.org/pubs/journals/pac}{Peace and Conflict: Journal of \newline Peace Psychology}</t>
   </si>
   <si>
     <t xml:space="preserve">\href{http://sumapsicologica.konradlorenz.edu.co/}{Summa Psicológica}</t>
@@ -714,7 +717,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScale="100" workbookViewId="0">
       <selection activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -800,7 +803,7 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -840,7 +843,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -951,46 +954,46 @@
     </row>
     <row r="21">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" ht="28.5">
+    <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" ht="28.5">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="24" ht="28.5">
+      <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1000,7 +1003,9 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1"/>
@@ -1022,6 +1027,13 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Added data editor procb and yupa supervision
</commit_message>
<xml_diff>
--- a/data/service_en.xlsx
+++ b/data/service_en.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t xml:space="preserve">what</t>
   </si>
@@ -37,6 +37,27 @@
     <t xml:space="preserve">why</t>
   </si>
   <si>
+    <t xml:space="preserve">Data Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\href{https://royalsocietypublishing.org/journal/rspb}{Proceedings of the Royal Society B}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editorial team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensuring compliance with data and code sharing standards prior to acceptance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifying that datasets, code, and materials are complete, accessible, and consistent with reported results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advising authors on adjustments needed to meet open data policies</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recommender (equivalent to Associate Editor)</t>
   </si>
   <si>
@@ -80,9 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">\href{https://www.frontiersin.org/journals/psychology}{Frontiers in Psychology}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editorial team</t>
   </si>
   <si>
     <t xml:space="preserve">Specialty section on \href{https://www.frontiersin.org/journals/psychology/sections/evolutionary-psychology}{Evolutionary Psychology}</t>
@@ -110,35 +128,7 @@
     <t xml:space="preserve">\href{https://royalsocietypublishing.org/journal/rspb}{Proceedings of the Royal Society B: \newline Biological Sciences}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">\href{https://royalsocietypublishing.org/journal/rstb}{Philosophical Transactions of the Royal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">\newline </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Society B: Biological Sciences}</t>
-    </r>
+    <t xml:space="preserve">\href{https://royalsocietypublishing.org/journal/rstb}{Philosophical Transactions of the Royal \newline Society B: Biological Sciences}</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -239,7 +229,8 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,20 +275,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,347 +485,383 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="109"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="109"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2" t="s">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>33</v>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>34</v>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>35</v>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>19</v>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>41</v>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>42</v>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>44</v>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="1" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
+    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" display="https://nyaspubs.onlinelibrary.wiley.com/journal/17496632"/>
+    <hyperlink ref="E15" r:id="rId1" display="\href{https://nyaspubs.onlinelibrary.wiley.com/journal/17496632}{Annals of the New York Academy of Sciences}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>